<commit_message>
added Locale:Armenian in the data set and picks as expected.
</commit_message>
<xml_diff>
--- a/src/main/resources/files/test_data.xlsx
+++ b/src/main/resources/files/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali.mulondo.PRUDENTIAL\Downloads\batch-extension-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41F656-3A65-4B37-B9C3-272C03031FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC256C1-B064-4E09-8535-5DB3AEB7C0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{248D7CD9-A2ED-4DF9-99F2-EB174E9DFB7C}"/>
   </bookViews>
@@ -33,9 +33,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Locale:Armenian</t>
+  </si>
+  <si>
+    <t>Locale: English(Uganda)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,13 +72,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -83,16 +118,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -413,159 +455,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00F9A04-3ECC-4114-9745-2D962CA6D9D8}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.7265625" customWidth="1"/>
+    <col min="2" max="2" width="35.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>44361</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+      <c r="B2" s="2">
+        <v>42408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>44592</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="B3" s="2">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>44216</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="B4" s="2">
+        <v>42296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>44543</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
+      <c r="B5" s="3">
+        <v>43020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
         <v>7338</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="B6" s="3">
+        <v>44226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>44501</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+      <c r="B7" s="2">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>43819</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="B8" s="2">
+        <v>43262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>44656</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="B9" s="2">
+        <v>43276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>44144</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="B10" s="2">
+        <v>42909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>44516</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="B11" s="2">
+        <v>43251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
         <v>44873</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+      <c r="B12" s="2">
+        <v>43565</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>43920</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="B13" s="2">
+        <v>43495</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>409468</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="B14" s="2">
+        <v>43332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>44238</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="B15" s="2">
+        <v>42415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
         <v>44847</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
+      <c r="B16" s="2">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>44627</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
+      <c r="B17" s="2">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>44468</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+      <c r="B18" s="2">
+        <v>43332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>44595</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+      <c r="B19" s="2">
+        <v>42853</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>44599</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+      <c r="B20" s="2">
+        <v>42853</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
         <v>44792</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="B21" s="2">
+        <v>43509</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
         <v>43894</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>43892</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>43277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>43892</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23" s="2">
+        <v>43166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
+        <v>43892</v>
+      </c>
+      <c r="B24" s="2">
+        <v>43304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
         <v>44474</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
+      <c r="B25" s="2">
+        <v>43140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
         <v>44762</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
+      <c r="B26" s="2">
+        <v>43367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
         <v>44595</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
+      <c r="B27" s="2">
+        <v>43633</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
         <v>44175</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
+      <c r="B28" s="2">
+        <v>43367</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
         <v>43907</v>
       </c>
+      <c r="B29" s="2">
+        <v>43633</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A28">
+  <conditionalFormatting sqref="A2:A29">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"if(len(E191)&lt;&gt;10)"</formula>
     </cfRule>

</xml_diff>